<commit_message>
Redone and Added heuristic succesfully
heuristic finds best initial seed for lab placements
</commit_message>
<xml_diff>
--- a/data/data_lunch_lab_allocated.xlsx
+++ b/data/data_lunch_lab_allocated.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4_CSE_C, 4_CSE_D, 4_AIDS_F, 4_CSBT_I, 4_IT_L, 4_ICT_M, 4_CSBS_N, 6_CSE_B, 6_CSE_C, 6_CSE_D, 6_CSE_E, 6_CSBT_I, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_E, 4_AIDS_H, 4_CSBT_I, 4_IT_K, 4_ICT_M, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_CSE_E, 6_AIDS_F, 6_AIDS_H, 6_IT_L</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_CSE_E, 4_AIDS_G, 4_AIDS_H, 4_IoTA_J, 4_IT_K, 6_CSE_A, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
+          <t>4_CSE_A, 4_CSE_D, 4_AIDS_F, 4_AIDS_G, 4_IoTA_J, 4_IT_L, 6_CSE_A, 6_CSE_C, 6_AIDS_G, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_D, 4_CSE_E, 4_AIDS_G, 4_AIDS_H, 4_IT_K, 4_IT_L, 4_ICT_M, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_D, 6_AIDS_G, 6_CSBT_I</t>
+          <t>4_CSE_B, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_IT_K, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IoTA_J, 6_IT_K</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_C, 4_AIDS_F, 4_CSBT_I, 4_IoTA_J, 6_CSE_B, 6_CSE_E, 6_AIDS_F, 6_AIDS_H, 6_IoTA_J, 6_IT_K, 6_IT_L, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_CSE_C, 4_CSE_D, 4_CSE_E, 4_CSBT_I, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_C, 6_AIDS_H, 6_IT_L, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_CSE_C, 4_CSE_D, 4_CSE_E, 4_IoTA_J, 4_IT_K, 4_IT_L, 6_CSE_B, 6_AIDS_H, 6_IoTA_J, 6_IT_L, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_CSBT_I, 4_IT_K, 4_IT_L, 4_CSBS_N, 6_CSE_E, 6_IoTA_J, 6_IT_K, 6_IT_L, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_ICT_M, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_D, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IT_K</t>
+          <t>4_CSE_A, 4_CSE_D, 4_AIDS_H, 4_IoTA_J, 4_ICT_M, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_D, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_CSBT_I, 6_ICT_M</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -724,7 +724,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4_CSE_C, 4_CSE_D, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_IT_K, 4_ICT_M, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_AIDS_F, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
+          <t>4_CSE_A, 4_CSE_B, 4_CSE_C, 4_CSE_D, 4_AIDS_F, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_C, 6_CSBT_I, 6_IoTA_J, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_IT_L, 4_CSBS_N, 6_CSE_D, 6_CSE_E, 6_AIDS_G, 6_AIDS_H, 6_CSBT_I, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_E, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_IT_K, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_IT_K, 6_IT_L</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_CSBS_N, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_IT_K, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_CSE_D, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_IT_L, 6_CSE_A, 6_CSE_C, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_CSBT_I, 6_ICT_M</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4_CSE_C, 4_CSE_D, 4_CSE_E, 4_IT_K, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_D, 6_CSBT_I, 6_IoTA_J, 6_IT_L, 6_ICT_M</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_E, 4_AIDS_F, 4_IT_K, 4_ICT_M, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_CSE_E, 6_IoTA_J, 6_IT_K, 6_IT_L, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>(1, 2), (1, 3)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(1, 4), (1, 5)</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>(1, 2), (1, 3)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>(4, 4), (4, 5)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(1, 2), (1, 3)</t>
         </is>
       </c>
     </row>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>(2, 2), (2, 3)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>(2, 2), (2, 3)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>(1, 2), (1, 3)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Done fixing staff conflicts in lab alloc
</commit_message>
<xml_diff>
--- a/data/data_lunch_lab_allocated.xlsx
+++ b/data/data_lunch_lab_allocated.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_CSE_C, 4_CSE_D, 4_CSE_E, 4_AIDS_H, 4_IoTA_J, 4_IT_K, 4_IT_L, 4_ICT_M, 6_CSE_C, 6_CSE_D, 6_AIDS_H, 6_IT_L</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_CSE_E, 4_IoTA_J, 4_IT_K, 4_IT_L, 6_CSE_A, 6_CSE_D, 6_CSE_E, 6_AIDS_G, 6_AIDS_H, 6_IT_K, 6_ICT_M</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4_AIDS_F, 4_AIDS_G, 4_CSBT_I, 4_CSBS_N, 6_CSE_A, 6_CSE_B, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_ICT_M, 4_CSBS_N, 6_CSE_B, 6_CSE_C, 6_AIDS_F, 6_CSBT_I, 6_IoTA_J, 6_IT_L, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_D, 4_IT_K, 4_IT_L, 4_ICT_M, 6_CSE_B, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_IT_L, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_D, 6_AIDS_H, 6_IoTA_J, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_C, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_D, 6_AIDS_H, 6_ICT_M</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_IoTA_J, 4_IT_K, 4_IT_L, 4_ICT_M, 6_CSE_B, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IT_K, 6_IT_L</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_AIDS_F, 4_AIDS_H, 4_IoTA_J, 4_ICT_M, 4_CSBS_N, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_CSBT_I, 6_IoTA_J, 6_IT_L</t>
+          <t>4_CSE_A, 4_CSE_B, 4_CSE_D, 4_AIDS_F, 4_AIDS_G, 4_IT_K, 4_CSBS_N, 6_CSE_A, 6_CSE_B, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_E, 4_AIDS_G, 4_CSBT_I, 4_IT_K, 4_IT_L, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_D, 6_CSE_E, 6_IT_K, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_C, 4_CSE_E, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_C, 6_CSE_D, 6_CSE_E, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -724,7 +724,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_C, 4_AIDS_G, 4_CSBT_I, 4_IT_K, 4_CSBS_N, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_D, 6_AIDS_F, 6_AIDS_G, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_CSE_C, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_ICT_M, 6_CSE_B, 6_CSE_D, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IT_K, 6_IT_L, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_D, 4_CSE_E, 4_AIDS_F, 4_AIDS_H, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_E, 6_AIDS_H, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
+          <t>4_CSE_B, 4_CSE_D, 4_CSE_E, 4_AIDS_F, 4_IoTA_J, 4_IT_K, 4_IT_L, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_E, 6_AIDS_H, 6_IoTA_J, 6_ICT_M</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_CSBT_I, 4_IT_L, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_E, 6_CSBT_I, 6_IT_K, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_C, 4_CSE_D, 4_AIDS_H, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_C, 6_CSE_E, 6_AIDS_F, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_C, 4_CSE_D, 4_AIDS_H, 4_IoTA_J, 4_IT_K, 4_ICT_M, 6_CSE_B, 6_CSE_D, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_IoTA_J, 6_IT_L</t>
+          <t>4_CSE_A, 4_CSE_B, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_CSBT_I, 4_IT_K, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_AIDS_G, 6_AIDS_H, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>(3, 0), (3, 1)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>(3, 0), (3, 1)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>(2, 2), (2, 3)</t>
+          <t>(1, 4), (1, 5)</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(1, 4), (1, 5)</t>
         </is>
       </c>
     </row>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>(2, 2), (2, 3)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(1, 2), (1, 3)</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>(4, 4), (4, 5)</t>
+          <t>(1, 4), (1, 5)</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>(1, 2), (1, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(1, 4), (1, 5)</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>(4, 4), (4, 5)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modularized mutation with and without classical optim
</commit_message>
<xml_diff>
--- a/data/data_lunch_lab_allocated.xlsx
+++ b/data/data_lunch_lab_allocated.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_CSE_E, 4_IoTA_J, 4_IT_K, 4_IT_L, 6_CSE_A, 6_CSE_D, 6_CSE_E, 6_AIDS_G, 6_AIDS_H, 6_IT_K, 6_ICT_M</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_E, 6_AIDS_F, 6_AIDS_H, 6_IoTA_J</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_ICT_M, 4_CSBS_N, 6_CSE_B, 6_CSE_C, 6_AIDS_F, 6_CSBT_I, 6_IoTA_J, 6_IT_L, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_CSE_D, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_IT_K, 4_CSBS_N, 6_CSE_D, 6_AIDS_G, 6_CSBT_I, 6_IT_K, 6_IT_L, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_D, 6_AIDS_H, 6_IoTA_J, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_AIDS_F, 4_AIDS_H, 4_CSBT_I, 4_IT_K, 4_IT_L, 4_ICT_M, 4_CSBS_N, 6_AIDS_F, 6_IT_K, 6_IT_L, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_IoTA_J, 4_IT_K, 4_IT_L, 4_ICT_M, 6_CSE_B, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IT_K, 6_IT_L</t>
+          <t>4_CSE_A, 4_CSE_E, 4_AIDS_G, 4_IoTA_J, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_D, 6_CSE_E, 6_AIDS_G, 6_AIDS_H, 6_CSBT_I, 6_IoTA_J, 6_ICT_M</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_CSE_D, 4_AIDS_F, 4_AIDS_G, 4_IT_K, 4_CSBS_N, 6_CSE_A, 6_CSE_B, 6_AIDS_F, 6_AIDS_G, 6_AIDS_H, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_A, 4_CSE_B, 4_CSE_C, 4_AIDS_F, 4_IoTA_J, 4_ICT_M, 6_CSE_A, 6_CSE_C, 6_CSE_E, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IT_L, 6_ICT_M</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4_CSE_C, 4_CSE_E, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_C, 6_CSE_D, 6_CSE_E, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
+          <t>4_CSE_D, 4_CSE_E, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_IT_K, 4_IT_L, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_AIDS_H, 6_IoTA_J, 6_IT_K, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -724,7 +724,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_C, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_ICT_M, 6_CSE_B, 6_CSE_D, 6_AIDS_F, 6_AIDS_G, 6_CSBT_I, 6_IT_K, 6_IT_L, 6_CSBS_N</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_AIDS_G, 4_IoTA_J, 4_CSBS_N, 6_CSE_C, 6_CSE_D, 6_AIDS_G, 6_AIDS_H, 6_IT_K, 6_IT_L, 6_ICT_M, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4_CSE_B, 4_CSE_D, 4_CSE_E, 4_AIDS_F, 4_IoTA_J, 4_IT_K, 4_IT_L, 4_CSBS_N, 6_CSE_A, 6_CSE_C, 6_CSE_E, 6_AIDS_H, 6_IoTA_J, 6_ICT_M</t>
+          <t>4_CSE_A, 4_CSE_E, 4_AIDS_F, 4_AIDS_H, 4_CSBT_I, 4_IT_K, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_B, 6_CSE_E, 6_AIDS_F, 6_CSBT_I, 6_IoTA_J</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4_CSE_C, 4_CSE_D, 4_AIDS_H, 4_IoTA_J, 4_IT_L, 4_ICT_M, 6_CSE_A, 6_CSE_C, 6_CSE_E, 6_AIDS_F, 6_CSBT_I, 6_IoTA_J, 6_IT_K, 6_IT_L</t>
+          <t>4_CSE_A, 4_CSE_E, 4_AIDS_G, 4_AIDS_H, 4_CSBT_I, 4_IoTA_J, 4_IT_K, 4_IT_L, 4_CSBS_N, 6_CSE_D, 6_AIDS_G, 6_AIDS_H, 6_CSBT_I, 6_CSBS_N</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4_CSE_A, 4_CSE_B, 4_CSE_E, 4_AIDS_F, 4_AIDS_G, 4_CSBT_I, 4_IT_K, 4_CSBS_N, 6_CSE_B, 6_CSE_D, 6_AIDS_G, 6_AIDS_H, 6_ICT_M, 6_CSBS_N</t>
+          <t>4_CSE_B, 4_CSE_C, 4_CSE_D, 4_AIDS_F, 4_ICT_M, 6_CSE_A, 6_CSE_B, 6_CSE_C, 6_CSE_E, 6_AIDS_F, 6_IoTA_J, 6_IT_K, 6_IT_L, 6_ICT_M</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(4, 2), (4, 3)</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>(3, 0), (3, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>(4, 4), (4, 5)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(4, 0), (4, 1)</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(1, 2), (1, 3)</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>(3, 0), (3, 1)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(0, 6), (0, 7)</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(2, 2), (2, 3)</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>(4, 0), (4, 1)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>(4, 4), (4, 5)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>(1, 0), (1, 1)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>(0, 4), (0, 5)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>(0, 6), (0, 7)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(0, 4), (0, 5)</t>
         </is>
       </c>
     </row>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(2, 4), (2, 5)</t>
         </is>
       </c>
     </row>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>(2, 0), (2, 1)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>(2, 2), (2, 3)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>(4, 2), (4, 3)</t>
+          <t>(0, 0), (0, 1)</t>
         </is>
       </c>
     </row>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>(2, 2), (2, 3)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>(3, 6), (3, 7)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>(4, 6), (4, 7)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>(3, 4), (3, 5)</t>
+          <t>(3, 2), (3, 3)</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(1, 4), (1, 5)</t>
         </is>
       </c>
     </row>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(4, 4), (4, 5)</t>
         </is>
       </c>
     </row>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>(1, 6), (1, 7)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(2, 0), (2, 1)</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 0), (3, 1)</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>(1, 4), (1, 5)</t>
+          <t>(1, 0), (1, 1)</t>
         </is>
       </c>
     </row>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>(2, 4), (2, 5)</t>
+          <t>(0, 2), (0, 3)</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>(0, 2), (0, 3)</t>
+          <t>(2, 6), (2, 7)</t>
         </is>
       </c>
     </row>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>(4, 4), (4, 5)</t>
+          <t>(1, 6), (1, 7)</t>
         </is>
       </c>
     </row>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>(3, 2), (3, 3)</t>
+          <t>(3, 6), (3, 7)</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>(0, 0), (0, 1)</t>
+          <t>(3, 4), (3, 5)</t>
         </is>
       </c>
     </row>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>(2, 6), (2, 7)</t>
+          <t>(4, 6), (4, 7)</t>
         </is>
       </c>
     </row>

</xml_diff>